<commit_message>
Issue #16: Update to remove Search Engines from the ranking.
</commit_message>
<xml_diff>
--- a/docs/popular-dbs.xlsx
+++ b/docs/popular-dbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/db-mining/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB59B8D9-FA94-EF4C-9A52-187F845195D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA334727-F4DA-4D40-840B-92E65E4943D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="24700" windowHeight="16560" activeTab="1" xr2:uid="{F3ED27E5-C21F-BB4B-A978-0CE0FDD733D7}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="25560" windowHeight="16560" activeTab="1" xr2:uid="{F3ED27E5-C21F-BB4B-A978-0CE0FDD733D7}"/>
   </bookViews>
   <sheets>
     <sheet name="v0 (old)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="107">
   <si>
     <t>DB Name</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>21 StackOverflow INTERSECT 21 DB-Engine</t>
+  </si>
+  <si>
+    <t>Netezza</t>
+  </si>
+  <si>
+    <t>Firebird</t>
+  </si>
+  <si>
+    <t>Neo4J</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +438,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -490,7 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -510,6 +530,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1127,7 +1150,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -1785,7 +1808,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Stack Overflow x DB-Engines'!$G$43:$G$49</c:f>
+              <c:f>'Stack Overflow x DB-Engines'!$G$45:$G$51</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1814,7 +1837,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stack Overflow x DB-Engines'!$H$43:$H$49</c:f>
+              <c:f>'Stack Overflow x DB-Engines'!$H$45:$H$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1831,7 +1854,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
@@ -2477,7 +2500,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Stack Overflow x DB-Engines'!$G$77:$G$83</c:f>
+              <c:f>'Stack Overflow x DB-Engines'!$G$80:$G$86</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2506,7 +2529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stack Overflow x DB-Engines'!$H$77:$H$83</c:f>
+              <c:f>'Stack Overflow x DB-Engines'!$H$80:$H$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2520,7 +2543,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -4326,13 +4349,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4364,13 +4387,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5252,10 +5275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE997D4E-A64F-234E-B719-2ED1C33C14C0}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5269,32 +5292,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -5332,29 +5355,31 @@
       <c r="E5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="22">
-        <f>COUNTIF($E$5:$E$36,G5)</f>
-        <v>19</v>
+      <c r="G5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="21">
+        <f>COUNTIF($E$5:$E$38,G5)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="22">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H6">
-        <f>COUNTIF($E$5:$E$36,G6)</f>
+      <c r="H6" s="24">
+        <f>COUNTIF($E$5:$E$38,G6)</f>
         <v>4</v>
       </c>
     </row>
@@ -5377,8 +5402,8 @@
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
-        <f>COUNTIF($E$5:$E$36,G7)</f>
+      <c r="H7" s="24">
+        <f>COUNTIF($E$5:$E$38,G7)</f>
         <v>2</v>
       </c>
     </row>
@@ -5401,8 +5426,8 @@
       <c r="G8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H8">
-        <f>COUNTIF($E$5:$E$36,G8)</f>
+      <c r="H8" s="24">
+        <f>COUNTIF($E$5:$E$38,G8)</f>
         <v>1</v>
       </c>
     </row>
@@ -5425,8 +5450,8 @@
       <c r="G9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H9">
-        <f>COUNTIF($E$5:$E$36,G9)</f>
+      <c r="H9" s="24">
+        <f>COUNTIF($E$5:$E$38,G9)</f>
         <v>1</v>
       </c>
     </row>
@@ -5449,13 +5474,14 @@
       <c r="G10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H10">
-        <f>COUNTIF($E$5:$E$36,G10)</f>
+      <c r="H10" s="24">
+        <f>COUNTIF($E$5:$E$38,G10)</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="5" t="s">
         <v>78</v>
       </c>
@@ -5468,8 +5494,8 @@
       <c r="G11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H11">
-        <f>COUNTIF($E$5:$E$36,G11)</f>
+      <c r="H11" s="26">
+        <f>COUNTIF($E$5:$E$38,G11)</f>
         <v>1</v>
       </c>
     </row>
@@ -5489,16 +5515,17 @@
       <c r="E12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="25">
         <f>SUM(H5:H11)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
         <v>71</v>
       </c>
@@ -5510,74 +5537,73 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>20</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="5">
-        <v>28</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="27">
+        <v>32</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="5">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="22">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="5">
         <v>6</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="C17" s="5" t="s">
+      <c r="E17" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="5">
         <v>27</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="5">
-        <v>13</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>11</v>
@@ -5585,531 +5611,549 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="5">
+        <v>13</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="5">
         <v>26</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="C20" s="5" t="s">
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="29"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D21" s="5">
         <v>9</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="E21" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>10</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D22" s="5">
         <v>24</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="C22" s="5" t="s">
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D23" s="5">
         <v>25</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>4</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="5">
-        <v>5</v>
-      </c>
       <c r="E23" s="10" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="5">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>3</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4</v>
-      </c>
-      <c r="E27" s="10" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="27">
+        <v>31</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
+        <v>9</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>6</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D30" s="5">
         <v>8</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="C29" s="5" t="s">
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="29"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D31" s="5">
         <v>20</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="C30" s="5" t="s">
+      <c r="E31" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="29"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D32" s="5">
         <v>21</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="11" t="s">
+      <c r="E32" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="29"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D33" s="11">
         <v>16</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E33" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="11" t="s">
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="29"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D34" s="11">
         <v>12</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E34" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <v>2</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D35" s="5">
         <v>3</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="E35" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <v>5</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="5">
-        <v>11</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C35" s="5" t="s">
+      <c r="D36" s="5">
+        <v>11</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D37" s="5">
         <v>15</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C36" s="5" t="s">
+      <c r="E37" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D38" s="5">
         <v>29</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="18" t="s">
+      <c r="D43" s="16"/>
+      <c r="E43" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
-        <v>13</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="5">
-        <v>18</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="22">
-        <f>COUNTIF($E$43:$E$70,G43)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
-        <v>14</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H44" s="25">
-        <f>COUNTIF($E$43:$E$70,G44)</f>
-        <v>3</v>
-      </c>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
+        <v>13</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="5">
         <v>18</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
       <c r="E45" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="25">
-        <f>COUNTIF($E$43:$E$70,G45)</f>
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="21">
+        <f>COUNTIF($E$45:$E$73,G45)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="5">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H46" s="25">
-        <f>COUNTIF($E$43:$E$70,G46)</f>
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="H46" s="24">
+        <f>COUNTIF($E$45:$E$73,G46)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="5">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" s="25">
-        <f>COUNTIF($E$43:$E$70,G47)</f>
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="H47" s="24">
+        <f>COUNTIF($E$45:$E$73,G47)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D48" s="5">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H48" s="25">
-        <f>COUNTIF($E$43:$E$70,G48)</f>
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="H48" s="24">
+        <f>COUNTIF($E$45:$E$73,G48)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D49" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="24">
+        <f>COUNTIF($E$45:$E$73,G49)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>15</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="5">
+        <v>10</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" s="24">
+        <f>COUNTIF($E$45:$E$73,G50)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="27">
+        <v>23</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H49" s="25">
-        <f>COUNTIF($E$43:$E$70,G49)</f>
+      <c r="H51" s="24">
+        <f>COUNTIF($E$45:$E$73,G51)</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="C50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D50" s="5">
-        <v>17</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="H50" s="20">
-        <f>SUM(H43:H49)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
-        <v>20</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="5">
+        <v>7</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>96</v>
+        <v>51</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52" s="19">
+        <f>SUM(H45:H51)</f>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
-        <v>16</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="A53" s="29"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D53" s="5">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>11</v>
@@ -6117,41 +6161,42 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="5">
-        <v>13</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
       <c r="E54" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
       <c r="E55" s="10" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
+      <c r="A56" s="5">
+        <v>16</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="C56" s="5" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D56" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>11</v>
@@ -6159,46 +6204,42 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="5">
+        <v>13</v>
+      </c>
       <c r="E57" s="10" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" s="5">
-        <v>5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
       <c r="E58" s="10" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="5">
-        <v>1</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A59" s="29"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="5" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D59" s="5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>11</v>
@@ -6206,46 +6247,46 @@
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
       <c r="E60" s="10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D61" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D62" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>11</v>
@@ -6253,500 +6294,568 @@
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
+        <v>17</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="27">
+        <v>22</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>9</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>3</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="5">
+        <v>4</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
         <v>6</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D66" s="5">
         <v>8</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E66" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="C64" s="5" t="s">
+    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="29"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D67" s="5">
         <v>20</v>
       </c>
-      <c r="E64" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="C65" s="5" t="s">
+      <c r="E67" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="29"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D68" s="5">
         <v>21</v>
       </c>
-      <c r="E65" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="11" t="s">
+      <c r="E68" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="29"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D66" s="11">
+      <c r="D69" s="11">
         <v>16</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E69" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="11"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="11" t="s">
+    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="29"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D67" s="11">
+      <c r="D70" s="11">
         <v>12</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E70" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
         <v>2</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D71" s="5">
         <v>3</v>
       </c>
-      <c r="E68" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="5">
+      <c r="E71" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
         <v>5</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D69" s="5">
-        <v>11</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C70" s="5" t="s">
+      <c r="D72" s="5">
+        <v>11</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="28"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D73" s="5">
         <v>15</v>
       </c>
-      <c r="E70" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="14" t="s">
+      <c r="E73" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-    </row>
-    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+    </row>
+    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17" t="s">
+      <c r="B78" s="16"/>
+      <c r="C78" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="18" t="s">
+      <c r="D78" s="16"/>
+      <c r="E78" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="G78" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D79" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="5">
-        <v>13</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D77" s="5">
-        <v>18</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G77" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H77" s="22">
-        <f>COUNTIF($E$77:$E$90,G77)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="5">
-        <v>21</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="5">
-        <v>19</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H78" s="25">
-        <f>COUNTIF($E$77:$E$90,G78)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="5">
-        <v>19</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D79" s="5">
-        <v>14</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H79" s="25">
-        <f>COUNTIF($E$77:$E$90,G79)</f>
-        <v>2</v>
-      </c>
+      <c r="E79" s="9"/>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D80" s="5">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H80" s="25">
-        <f>COUNTIF($E$77:$E$90,G80)</f>
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" s="21">
+        <f>COUNTIF($E$80:$E$94,G80)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D81" s="5">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E81" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G81" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H81" s="25">
-        <f>COUNTIF($E$77:$E$90,G81)</f>
-        <v>1</v>
+      <c r="H81" s="24">
+        <f>COUNTIF($E$80:$E$94,G81)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D82" s="5">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H82" s="25">
-        <f>COUNTIF($E$77:$E$90,G82)</f>
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="H82" s="24">
+        <f>COUNTIF($E$80:$E$94,G82)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D83" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H83" s="27">
-        <f>COUNTIF($E$77:$E$90,G83)</f>
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="H83" s="24">
+        <f>COUNTIF($E$80:$E$94,G83)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D84" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E84" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G84" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G84" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="H84" s="26">
-        <f>SUM(H77:H83)</f>
-        <v>14</v>
+      <c r="H84" s="24">
+        <f>COUNTIF($E$80:$E$94,G84)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
+        <v>16</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" s="5">
+        <v>6</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H85" s="24">
+        <f>COUNTIF($E$80:$E$94,G85)</f>
         <v>1</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D85" s="5">
-        <v>2</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D86" s="5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>11</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H86" s="26">
+        <f>COUNTIF($E$80:$E$94,G86)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D87" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H87" s="25">
+        <f>SUM(H80:H86)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D88" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D89" s="5">
-        <v>3</v>
+        <v>106</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89" s="27">
+        <v>22</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
+        <v>9</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D90" s="5">
+        <v>1</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>3</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" s="5">
+        <v>4</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>6</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D92" s="5">
+        <v>8</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
+        <v>2</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D93" s="5">
+        <v>3</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
         <v>5</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B94" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D90" s="5">
-        <v>11</v>
-      </c>
-      <c r="E90" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="10"/>
-    </row>
-    <row r="92" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="23"/>
-      <c r="C92" s="23"/>
-      <c r="D92" s="23"/>
-      <c r="E92" s="24"/>
-    </row>
-    <row r="93" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="23"/>
-      <c r="C93" s="23"/>
-      <c r="D93" s="23"/>
-      <c r="E93" s="24"/>
-    </row>
-    <row r="104" spans="3:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="10"/>
+      <c r="D94" s="5">
+        <v>11</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="22"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="23"/>
+    </row>
+    <row r="96" spans="1:8" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="22"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="23"/>
+    </row>
+    <row r="107" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C22:D36">
-    <sortCondition ref="C22"/>
-  </sortState>
   <mergeCells count="9">
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:E79"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:E44"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Issue #16: Updates the list of databases using the 2019 ranking
</commit_message>
<xml_diff>
--- a/docs/popular-dbs.xlsx
+++ b/docs/popular-dbs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/db-mining/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA334727-F4DA-4D40-840B-92E65E4943D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75E6776-BE8D-ED45-BD23-D44F298CA586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="25560" windowHeight="16560" activeTab="1" xr2:uid="{F3ED27E5-C21F-BB4B-A978-0CE0FDD733D7}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="32320" windowHeight="19980" activeTab="2" xr2:uid="{F3ED27E5-C21F-BB4B-A978-0CE0FDD733D7}"/>
   </bookViews>
   <sheets>
     <sheet name="v0 (old)" sheetId="1" r:id="rId1"/>
-    <sheet name="Stack Overflow x DB-Engines" sheetId="2" r:id="rId2"/>
+    <sheet name="Stack Overflow 18 x DB-Engines" sheetId="2" r:id="rId2"/>
+    <sheet name="Stack Overflow 19 x DB-Engines" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="110">
   <si>
     <t>DB Name</t>
   </si>
@@ -353,6 +354,15 @@
   </si>
   <si>
     <t>Neo4J</t>
+  </si>
+  <si>
+    <t>Firebase</t>
+  </si>
+  <si>
+    <t>13 StackOverflow UNION 13 DB-Engine</t>
+  </si>
+  <si>
+    <t>13 StackOverflow INTERSECT 13 DB-Engine</t>
   </si>
 </sst>
 </file>
@@ -496,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -506,21 +516,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -533,6 +534,17 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1088,6 +1100,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1116,7 +1135,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Stack Overflow x DB-Engines'!$G$5:$G$11</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$G$5:$G$11</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1145,7 +1164,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stack Overflow x DB-Engines'!$H$5:$H$11</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$H$5:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1780,6 +1799,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1808,7 +1834,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Stack Overflow x DB-Engines'!$G$45:$G$51</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$G$45:$G$51</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1837,7 +1863,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stack Overflow x DB-Engines'!$H$45:$H$51</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$H$45:$H$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2472,6 +2498,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2500,7 +2533,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Stack Overflow x DB-Engines'!$G$80:$G$86</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$G$80:$G$86</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2529,7 +2562,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stack Overflow x DB-Engines'!$H$80:$H$86</c:f>
+              <c:f>'Stack Overflow 18 x DB-Engines'!$H$80:$H$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2560,6 +2593,1404 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-F4D4-E34B-B14E-327369CA406C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Types</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stack Overflow 19 x DB-Engines'!$G$5:$G$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Relational</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Multimodel</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Columnar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Graph</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Document</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Key-Value</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>File System</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stack Overflow 19 x DB-Engines'!$H$5:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-B1DA-CB4C-8E70-6BE3FBE36D11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Type</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-488D-EB49-9192-B4E60E354180}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-488D-EB49-9192-B4E60E354180}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stack Overflow 19 x DB-Engines'!$G$29:$G$35</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Relational</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Multimodel</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Columnar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Graph</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Document</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Key-Value</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>File System</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stack Overflow 19 x DB-Engines'!$H$29:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-488D-EB49-9192-B4E60E354180}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2747,6 +4178,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
   <cs:axisTitle>
@@ -3788,6 +5299,1046 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4416,6 +6967,87 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B463593D-2CAE-1F44-B8CB-35E9256694E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A439FBBF-D07C-C14B-A4DB-DBB03AA67629}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5277,7 +7909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE997D4E-A64F-234E-B719-2ED1C33C14C0}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -5292,32 +7924,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -5337,7 +7969,7 @@
       <c r="D4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
@@ -5352,34 +7984,34 @@
       <c r="D5" s="5">
         <v>18</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="21">
-        <f>COUNTIF($E$5:$E$38,G5)</f>
+      <c r="H5" s="18">
+        <f t="shared" ref="H5:H11" si="0">COUNTIF($E$5:$E$38,G5)</f>
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="19">
         <v>14</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="24">
-        <f>COUNTIF($E$5:$E$38,G6)</f>
+      <c r="H6" s="21">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -5396,14 +8028,14 @@
       <c r="D7" s="5">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="24">
-        <f>COUNTIF($E$5:$E$38,G7)</f>
+      <c r="H7" s="21">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -5420,14 +8052,14 @@
       <c r="D8" s="5">
         <v>19</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="24">
-        <f>COUNTIF($E$5:$E$38,G8)</f>
+      <c r="H8" s="21">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5444,14 +8076,14 @@
       <c r="D9" s="5">
         <v>14</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="24">
-        <f>COUNTIF($E$5:$E$38,G9)</f>
+      <c r="H9" s="21">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5468,34 +8100,34 @@
       <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="24">
-        <f>COUNTIF($E$5:$E$38,G10)</f>
+      <c r="H10" s="21">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D11" s="5">
         <v>23</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>51</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="26">
-        <f>COUNTIF($E$5:$E$38,G11)</f>
+      <c r="H11" s="23">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5512,40 +8144,40 @@
       <c r="D12" s="5">
         <v>7</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <f>SUM(H5:H11)</f>
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="5">
         <v>17</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="27" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="24">
         <v>32</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5562,20 +8194,20 @@
       <c r="D15" s="5">
         <v>28</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="22">
+      <c r="A16" s="19">
         <v>12</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="9" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5592,20 +8224,20 @@
       <c r="D17" s="5">
         <v>6</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="5">
         <v>27</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5622,7 +8254,7 @@
       <c r="D19" s="5">
         <v>13</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5639,20 +8271,20 @@
       <c r="D20" s="5">
         <v>26</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="5">
         <v>9</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5669,20 +8301,20 @@
       <c r="D22" s="5">
         <v>24</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D23" s="5">
         <v>25</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5699,7 +8331,7 @@
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5716,7 +8348,7 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5733,20 +8365,20 @@
       <c r="D26" s="5">
         <v>22</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="27" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="24">
         <v>31</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5763,7 +8395,7 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5780,7 +8412,7 @@
       <c r="D29" s="5">
         <v>4</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5797,59 +8429,59 @@
       <c r="D30" s="5">
         <v>8</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D31" s="5">
         <v>20</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D32" s="5">
         <v>21</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="11" t="s">
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="10">
         <v>16</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="11" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <v>12</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>97</v>
       </c>
     </row>
@@ -5866,7 +8498,7 @@
       <c r="D35" s="5">
         <v>3</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5883,68 +8515,68 @@
       <c r="D36" s="5">
         <v>11</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D37" s="5">
         <v>15</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D38" s="5">
         <v>29</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="23"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16" t="s">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="17" t="s">
+      <c r="D43" s="27"/>
+      <c r="E43" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G43" s="6" t="s">
@@ -5964,7 +8596,7 @@
       <c r="D44" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E44" s="9"/>
+      <c r="E44" s="29"/>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
@@ -5979,14 +8611,14 @@
       <c r="D45" s="5">
         <v>18</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="21">
-        <f>COUNTIF($E$45:$E$73,G45)</f>
+      <c r="H45" s="18">
+        <f t="shared" ref="H45:H51" si="1">COUNTIF($E$45:$E$73,G45)</f>
         <v>16</v>
       </c>
     </row>
@@ -5997,16 +8629,16 @@
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="10" t="s">
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H46" s="24">
-        <f>COUNTIF($E$45:$E$73,G46)</f>
+      <c r="H46" s="21">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6017,16 +8649,16 @@
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="10" t="s">
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H47" s="24">
-        <f>COUNTIF($E$45:$E$73,G47)</f>
+      <c r="H47" s="21">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -6043,14 +8675,14 @@
       <c r="D48" s="5">
         <v>19</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H48" s="24">
-        <f>COUNTIF($E$45:$E$73,G48)</f>
+      <c r="H48" s="21">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6067,14 +8699,14 @@
       <c r="D49" s="5">
         <v>14</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="24">
-        <f>COUNTIF($E$45:$E$73,G49)</f>
+      <c r="H49" s="21">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -6091,34 +8723,34 @@
       <c r="D50" s="5">
         <v>10</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H50" s="24">
-        <f>COUNTIF($E$45:$E$73,G50)</f>
+      <c r="H50" s="21">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="27" t="s">
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="27">
+      <c r="D51" s="24">
         <v>23</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H51" s="24">
-        <f>COUNTIF($E$45:$E$73,G51)</f>
+      <c r="H51" s="21">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6135,27 +8767,27 @@
       <c r="D52" s="5">
         <v>7</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="G52" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H52" s="19">
+      <c r="H52" s="16">
         <f>SUM(H45:H51)</f>
         <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
-      <c r="B53" s="28"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="25"/>
       <c r="C53" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D53" s="5">
         <v>17</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6166,9 +8798,9 @@
       <c r="B54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="10" t="s">
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6179,9 +8811,9 @@
       <c r="B55" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="10" t="s">
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="9" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6198,7 +8830,7 @@
       <c r="D56" s="5">
         <v>6</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6215,7 +8847,7 @@
       <c r="D57" s="5">
         <v>13</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6226,22 +8858,22 @@
       <c r="B58" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="10" t="s">
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="25"/>
       <c r="C59" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D59" s="5">
         <v>9</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6252,9 +8884,9 @@
       <c r="B60" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="10" t="s">
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6271,7 +8903,7 @@
       <c r="D61" s="5">
         <v>5</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6288,7 +8920,7 @@
       <c r="D62" s="5">
         <v>2</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6299,13 +8931,13 @@
       <c r="B63" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="C63" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D63" s="27">
+      <c r="D63" s="24">
         <v>22</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6322,7 +8954,7 @@
       <c r="D64" s="5">
         <v>1</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6339,7 +8971,7 @@
       <c r="D65" s="5">
         <v>4</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6356,59 +8988,59 @@
       <c r="D66" s="5">
         <v>8</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="E66" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D67" s="5">
         <v>20</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="29"/>
-      <c r="B68" s="28"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D68" s="5">
         <v>21</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="11" t="s">
+      <c r="A69" s="26"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D69" s="11">
+      <c r="D69" s="10">
         <v>16</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
-      <c r="B70" s="28"/>
-      <c r="C70" s="11" t="s">
+      <c r="A70" s="26"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="11">
+      <c r="D70" s="10">
         <v>12</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="11" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6425,7 +9057,7 @@
       <c r="D71" s="5">
         <v>3</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="E71" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6442,60 +9074,60 @@
       <c r="D72" s="5">
         <v>11</v>
       </c>
-      <c r="E72" s="10" t="s">
+      <c r="E72" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="28"/>
-      <c r="B73" s="28"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="25"/>
       <c r="C73" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D73" s="5">
         <v>15</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
-      <c r="E74" s="10"/>
+      <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
-      <c r="E75" s="10"/>
+      <c r="E75" s="9"/>
     </row>
     <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
     </row>
     <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16" t="s">
+      <c r="B78" s="27"/>
+      <c r="C78" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D78" s="16"/>
-      <c r="E78" s="17" t="s">
+      <c r="D78" s="27"/>
+      <c r="E78" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G78" s="6" t="s">
@@ -6515,7 +9147,7 @@
       <c r="D79" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E79" s="9"/>
+      <c r="E79" s="29"/>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
@@ -6530,14 +9162,14 @@
       <c r="D80" s="5">
         <v>18</v>
       </c>
-      <c r="E80" s="10" t="s">
+      <c r="E80" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G80" s="20" t="s">
+      <c r="G80" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H80" s="21">
-        <f>COUNTIF($E$80:$E$94,G80)</f>
+      <c r="H80" s="18">
+        <f t="shared" ref="H80:H86" si="2">COUNTIF($E$80:$E$94,G80)</f>
         <v>8</v>
       </c>
     </row>
@@ -6554,14 +9186,14 @@
       <c r="D81" s="5">
         <v>19</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H81" s="24">
-        <f>COUNTIF($E$80:$E$94,G81)</f>
+      <c r="H81" s="21">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -6578,14 +9210,14 @@
       <c r="D82" s="5">
         <v>14</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E82" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H82" s="24">
-        <f>COUNTIF($E$80:$E$94,G82)</f>
+      <c r="H82" s="21">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -6602,14 +9234,14 @@
       <c r="D83" s="5">
         <v>10</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H83" s="24">
-        <f>COUNTIF($E$80:$E$94,G83)</f>
+      <c r="H83" s="21">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6626,14 +9258,14 @@
       <c r="D84" s="5">
         <v>7</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="9" t="s">
         <v>51</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H84" s="24">
-        <f>COUNTIF($E$80:$E$94,G84)</f>
+      <c r="H84" s="21">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6650,14 +9282,14 @@
       <c r="D85" s="5">
         <v>6</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E85" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H85" s="24">
-        <f>COUNTIF($E$80:$E$94,G85)</f>
+      <c r="H85" s="21">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6674,14 +9306,14 @@
       <c r="D86" s="5">
         <v>13</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="E86" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H86" s="26">
-        <f>COUNTIF($E$80:$E$94,G86)</f>
+      <c r="H86" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6698,13 +9330,13 @@
       <c r="D87" s="5">
         <v>5</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E87" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G87" s="18" t="s">
+      <c r="G87" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H87" s="25">
+      <c r="H87" s="22">
         <f>SUM(H80:H86)</f>
         <v>15</v>
       </c>
@@ -6722,7 +9354,7 @@
       <c r="D88" s="5">
         <v>2</v>
       </c>
-      <c r="E88" s="10" t="s">
+      <c r="E88" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6733,13 +9365,13 @@
       <c r="B89" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="27" t="s">
+      <c r="C89" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D89" s="27">
+      <c r="D89" s="24">
         <v>22</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="E89" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6756,7 +9388,7 @@
       <c r="D90" s="5">
         <v>1</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E90" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6773,7 +9405,7 @@
       <c r="D91" s="5">
         <v>4</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6790,7 +9422,7 @@
       <c r="D92" s="5">
         <v>8</v>
       </c>
-      <c r="E92" s="10" t="s">
+      <c r="E92" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6807,7 +9439,7 @@
       <c r="D93" s="5">
         <v>3</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="E93" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6824,26 +9456,26 @@
       <c r="D94" s="5">
         <v>11</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="E94" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="22"/>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="23"/>
-    </row>
-    <row r="96" spans="1:8" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="22"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="23"/>
+    <row r="95" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="19"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="20"/>
+    </row>
+    <row r="96" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="19"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="20"/>
     </row>
     <row r="107" spans="3:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
-      <c r="E107" s="10"/>
+      <c r="E107" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6860,4 +9492,710 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C112D9A0-5D71-E246-98CE-F8B9C77D34A9}">
+  <dimension ref="A1:K55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
+    <col min="7" max="7" width="43.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="9"/>
+      <c r="G5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="18">
+        <f>COUNTIF($E$5:$E$22,G5)</f>
+        <v>9</v>
+      </c>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="24">
+        <v>14</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="21">
+        <f>COUNTIF($E$5:$E$22,G6)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="21">
+        <f>COUNTIF($E$5:$E$22,G7)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="31"/>
+      <c r="G8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="21">
+        <f>COUNTIF($E$5:$E$22,G8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="21">
+        <f>COUNTIF($E$5:$E$22,G9)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="21">
+        <f>COUNTIF($E$5:$E$22,G10)</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="5">
+        <v>6</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="23">
+        <f>COUNTIF($E$5:$E$22,G11)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="5">
+        <v>13</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="22">
+        <f>SUM(H5:H11)</f>
+        <v>14</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="26"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="10">
+        <v>12</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="5">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>12</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="5">
+        <v>10</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="18">
+        <f>COUNTIF($E$29:$E$42,G29)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="5">
+        <v>7</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="21">
+        <f>COUNTIF($E$29:$E$42,G30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>7</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="5">
+        <v>13</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="21">
+        <f>COUNTIF($E$29:$E$42,G31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="5">
+        <v>5</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="21">
+        <f>COUNTIF($E$29:$E$42,G32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="21">
+        <f>COUNTIF($E$29:$E$42,G33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>8</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="21">
+        <f>COUNTIF($E$29:$E$42,G34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>2</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" s="23">
+        <f>COUNTIF($E$29:$E$42,G35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>6</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="5">
+        <v>8</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="22">
+        <f>SUM(H29:H35)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="5">
+        <v>11</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>